<commit_message>
Time delay and lag 2 step optimization
</commit_message>
<xml_diff>
--- a/Benchmark_System/Time_Delay_and_lag2/Time Delay and Lag2.xlsx
+++ b/Benchmark_System/Time_Delay_and_lag2/Time Delay and Lag2.xlsx
@@ -152,16 +152,16 @@
         <v>1</v>
       </c>
       <c r="B2">
-        <v>1.3750898062689094</v>
+        <v>1.3750999659704599</v>
       </c>
       <c r="C2">
-        <v>3.4499011968914033</v>
+        <v>3.4500595774128766</v>
       </c>
       <c r="D2">
-        <v>1.6391459339231353</v>
+        <v>1.6391627272293354</v>
       </c>
       <c r="E2">
-        <v>1.5771616808384232</v>
+        <v>1.4912153409914097</v>
       </c>
     </row>
     <row r="3">
@@ -169,16 +169,16 @@
         <v>2</v>
       </c>
       <c r="B3">
-        <v>1.8388874440259555</v>
+        <v>1.839299632548925</v>
       </c>
       <c r="C3">
-        <v>0.57526906906400654</v>
+        <v>0.57421817686101884</v>
       </c>
       <c r="D3">
-        <v>1.9201887705579332</v>
+        <v>1.9248988078259972</v>
       </c>
       <c r="E3">
-        <v>1.2986845267101614</v>
+        <v>1.4168087968476042</v>
       </c>
     </row>
     <row r="4">
@@ -186,16 +186,16 @@
         <v>3</v>
       </c>
       <c r="B4">
-        <v>2.4109844542644598</v>
+        <v>2.4111537307867583</v>
       </c>
       <c r="C4">
-        <v>0.38225988125848548</v>
+        <v>0.38172367380654204</v>
       </c>
       <c r="D4">
-        <v>2.9975558737232175</v>
+        <v>3.0028397097794528</v>
       </c>
       <c r="E4">
-        <v>1.391592462655266</v>
+        <v>1.662715776824724</v>
       </c>
     </row>
     <row r="5">
@@ -203,16 +203,16 @@
         <v>4</v>
       </c>
       <c r="B5">
-        <v>0.3866462686292067</v>
+        <v>0.38704723084047982</v>
       </c>
       <c r="C5">
-        <v>14.700832773321284</v>
+        <v>14.85420109889974</v>
       </c>
       <c r="D5">
-        <v>0.37431617540509599</v>
+        <v>0.37570128233747402</v>
       </c>
       <c r="E5">
-        <v>0.52258720371386413</v>
+        <v>0.49193177896086732</v>
       </c>
     </row>
     <row r="6">
@@ -220,7 +220,7 @@
         <v>5</v>
       </c>
       <c r="E6">
-        <v>19.999923565770462</v>
+        <v>29.996407810101477</v>
       </c>
     </row>
     <row r="7">
@@ -262,16 +262,16 @@
         <v>8</v>
       </c>
       <c r="B9">
-        <v>32.995946006804523</v>
+        <v>32.978970526181556</v>
       </c>
       <c r="C9">
-        <v>3.0000934279380358</v>
+        <v>3.0000255431164389</v>
       </c>
       <c r="D9">
-        <v>32.996229611731671</v>
+        <v>32.974399796881222</v>
       </c>
       <c r="E9">
-        <v>32.993422868201186</v>
+        <v>32.981668565336498</v>
       </c>
     </row>
     <row r="10">
@@ -279,7 +279,7 @@
         <v>9</v>
       </c>
       <c r="E10">
-        <v>3.0001603189407873</v>
+        <v>3.0072943573859146</v>
       </c>
     </row>
     <row r="11">
@@ -287,16 +287,16 @@
         <v>10</v>
       </c>
       <c r="B11">
-        <v>0.72188479739857736</v>
+        <v>0.72125116029461611</v>
       </c>
       <c r="C11">
-        <v>1.3333856511461448</v>
+        <v>1.333666917992703</v>
       </c>
       <c r="D11">
-        <v>0.90631016319172808</v>
+        <v>0.90524422118296255</v>
       </c>
       <c r="E11">
-        <v>0.70845343228430924</v>
+        <v>0.72475219688574244</v>
       </c>
     </row>
     <row r="12">
@@ -304,16 +304,16 @@
         <v>11</v>
       </c>
       <c r="B12">
-        <v>3.9541860574943484</v>
+        <v>3.9540006386741626</v>
       </c>
       <c r="C12">
-        <v>17.363861820039784</v>
+        <v>17.423704598910113</v>
       </c>
       <c r="D12">
-        <v>4.4086586661330367</v>
+        <v>4.4077336711713668</v>
       </c>
       <c r="E12">
-        <v>9.4882535699166031</v>
+        <v>5.2485168304383238</v>
       </c>
     </row>
     <row r="13">
@@ -321,16 +321,16 @@
         <v>12</v>
       </c>
       <c r="B13">
-        <v>9.3758635810902149</v>
+        <v>9.4438898024387541</v>
       </c>
       <c r="C13">
-        <v>29.507866070430786</v>
+        <v>29.524046030795393</v>
       </c>
       <c r="D13">
-        <v>5.5036760532662266</v>
+        <v>5.5448721289041547</v>
       </c>
       <c r="E13">
-        <v>8.2141357491205991</v>
+        <v>8.4511642667044917</v>
       </c>
     </row>
     <row r="14">
@@ -341,7 +341,7 @@
         <v>-0</v>
       </c>
       <c r="C14">
-        <v>6.325997931428068e-15</v>
+        <v>8.1127857221791728e-15</v>
       </c>
       <c r="D14">
         <v>-0</v>
@@ -355,16 +355,16 @@
         <v>14</v>
       </c>
       <c r="B15">
-        <v>1.0937586358109022</v>
+        <v>1.0944388980243875</v>
       </c>
       <c r="C15">
-        <v>1.2950786607043079</v>
+        <v>1.2952404603079539</v>
       </c>
       <c r="D15">
-        <v>1.0550367896610309</v>
+        <v>1.0554488235124633</v>
       </c>
       <c r="E15">
-        <v>1.082141357491206</v>
+        <v>1.0845116426670449</v>
       </c>
     </row>
     <row r="16">
@@ -372,16 +372,16 @@
         <v>15</v>
       </c>
       <c r="B16">
-        <v>1.9877433723052274</v>
+        <v>1.9880341774986883</v>
       </c>
       <c r="C16">
-        <v>4.0833372719410024</v>
+        <v>4.0849543957641687</v>
       </c>
       <c r="D16">
-        <v>2.6717560570208665</v>
+        <v>2.6802684809369128</v>
       </c>
       <c r="E16">
-        <v>1.9605129290244971</v>
+        <v>1.9759349973543752</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
time delay and lag 2 corect Ta
</commit_message>
<xml_diff>
--- a/Benchmark_System/Time_Delay_and_lag2/Time Delay and Lag2.xlsx
+++ b/Benchmark_System/Time_Delay_and_lag2/Time Delay and Lag2.xlsx
@@ -1,19 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
+  <workbookPr defaultThemeVersion="166925"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dell\Documents\PID_PIDA_Controller\Benchmark_System\Time_Delay_and_lag2\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6FBB0D8-48E1-4F0D-9C43-203B4FB8503F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView activeTab="0"/>
+    <workbookView xWindow="240" yWindow="240" windowWidth="18840" windowHeight="15120" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId2"/>
+    <sheet name="Reference Tracking" sheetId="1" r:id="rId1"/>
+    <sheet name="Disturbance Rejection" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="125725" fullCalcOnLoad="true"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="20">
   <si>
     <t>parametri</t>
   </si>
@@ -78,8 +86,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <name val="Calibri"/>
@@ -93,7 +101,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -101,36 +109,349 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border/>
-    <border/>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normale" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema di Office">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="44546A"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="E7E6E6"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="4472C4"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="ED7D31"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="A5A5A5"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="FFC000"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="5B9BD5"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="70AD47"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0563C1"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="954F72"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック Light"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线 Light"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="110000"/>
+                <a:satMod val="105000"/>
+                <a:tint val="67000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="103000"/>
+                <a:tint val="73000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="109000"/>
+                <a:tint val="81000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:satMod val="103000"/>
+                <a:lumMod val="102000"/>
+                <a:tint val="94000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:satMod val="110000"/>
+                <a:lumMod val="100000"/>
+                <a:shade val="100000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="99000"/>
+                <a:satMod val="120000"/>
+                <a:shade val="78000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="63000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:tint val="95000"/>
+            <a:satMod val="170000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="93000"/>
+                <a:satMod val="150000"/>
+                <a:shade val="98000"/>
+                <a:lumMod val="102000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:tint val="98000"/>
+                <a:satMod val="130000"/>
+                <a:shade val="90000"/>
+                <a:lumMod val="103000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="63000"/>
+                <a:satMod val="120000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+  <a:extLst>
+    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+    </a:ext>
+  </a:extLst>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E16"/>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetViews>
+    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection sqref="A1:E16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.140625" customWidth="true"/>
-    <col min="2" max="2" width="12.7109375" customWidth="true"/>
-    <col min="3" max="3" width="15.5703125" customWidth="true"/>
-    <col min="4" max="4" width="12.7109375" customWidth="true"/>
-    <col min="5" max="5" width="12.7109375" customWidth="true"/>
+    <col min="1" max="1" width="12.140625" customWidth="1"/>
+    <col min="2" max="2" width="12.7109375" customWidth="1"/>
+    <col min="3" max="3" width="15.5703125" customWidth="1"/>
+    <col min="4" max="5" width="12.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -147,7 +468,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -161,10 +482,10 @@
         <v>1.6357062607456536</v>
       </c>
       <c r="E2">
-        <v>1.3646447975327418</v>
-      </c>
-    </row>
-    <row r="3">
+        <v>1.3622267795840934</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
@@ -178,10 +499,10 @@
         <v>1.9344674126000521</v>
       </c>
       <c r="E3">
-        <v>1.8119677320226575</v>
-      </c>
-    </row>
-    <row r="4">
+        <v>1.8198662038490239</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
@@ -195,10 +516,10 @@
         <v>3.013610989990386</v>
       </c>
       <c r="E4">
-        <v>2.3393947173274188</v>
-      </c>
-    </row>
-    <row r="5">
+        <v>2.3440647863010766</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
@@ -212,18 +533,18 @@
         <v>0.37886362653014721</v>
       </c>
       <c r="E5">
-        <v>0.40772577522351194</v>
-      </c>
-    </row>
-    <row r="6">
+        <v>0.40912892935754369</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
       <c r="E6">
-        <v>299.88848293910587</v>
-      </c>
-    </row>
-    <row r="7">
+        <v>369.08323917404419</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>6</v>
       </c>
@@ -240,7 +561,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>7</v>
       </c>
@@ -257,7 +578,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>8</v>
       </c>
@@ -271,18 +592,18 @@
         <v>62.437884687648456</v>
       </c>
       <c r="E9">
-        <v>149.91763454899771</v>
-      </c>
-    </row>
-    <row r="10">
+        <v>420.81949491143354</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>9</v>
       </c>
       <c r="E10">
-        <v>3.0157637066176211</v>
-      </c>
-    </row>
-    <row r="11">
+        <v>3.2336185741314547</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>10</v>
       </c>
@@ -296,10 +617,10 @@
         <v>0.89986020512674303</v>
       </c>
       <c r="E11">
-        <v>0.69892522786619193</v>
-      </c>
-    </row>
-    <row r="12">
+        <v>0.69509171698977945</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>11</v>
       </c>
@@ -313,10 +634,10 @@
         <v>4.3890616420775332</v>
       </c>
       <c r="E12">
-        <v>3.9136930789354354</v>
-      </c>
-    </row>
-    <row r="13">
+        <v>3.9049148679741372</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>12</v>
       </c>
@@ -330,27 +651,27 @@
         <v>5.501490251486052</v>
       </c>
       <c r="E13">
-        <v>10.831518916432859</v>
-      </c>
-    </row>
-    <row r="14">
+        <v>11.194267208742215</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>13</v>
       </c>
       <c r="B14">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="C14">
-        <v>1.2563168873892269e-14</v>
+        <v>1.2563168873892269E-14</v>
       </c>
       <c r="D14">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="E14">
-        <v>-0</v>
-      </c>
-    </row>
-    <row r="15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>14</v>
       </c>
@@ -364,10 +685,10 @@
         <v>1.0550149070136141</v>
       </c>
       <c r="E15">
-        <v>1.1083151891643286</v>
-      </c>
-    </row>
-    <row r="16">
+        <v>1.1119426720874219</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>15</v>
       </c>
@@ -381,9 +702,210 @@
         <v>2.6488905298484036</v>
       </c>
       <c r="E16">
-        <v>1.9796830864600783</v>
+        <v>1.9795459877187256</v>
       </c>
     </row>
   </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{679C9229-F6F6-48D9-AA02-C149A9A9987B}">
+  <dimension ref="A1:E16"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>0.64092905868840899</v>
+      </c>
+      <c r="C2">
+        <v>0.64092445774446805</v>
+      </c>
+      <c r="D2">
+        <v>1.6357062607456536</v>
+      </c>
+      <c r="E2">
+        <v>1.3622267795840934</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>2.6565911685239598</v>
+      </c>
+      <c r="C3">
+        <v>0.575038314211061</v>
+      </c>
+      <c r="D3">
+        <v>1.9344674126000521</v>
+      </c>
+      <c r="E3">
+        <v>1.8198662038490239</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>1.39321831608833</v>
+      </c>
+      <c r="C4">
+        <v>0.38246634346068148</v>
+      </c>
+      <c r="D4">
+        <v>3.013610989990386</v>
+      </c>
+      <c r="E4">
+        <v>2.3440647863010766</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <v>0.44321713114331701</v>
+      </c>
+      <c r="C5">
+        <v>14.792613842859677</v>
+      </c>
+      <c r="D5">
+        <v>0.37886362653014721</v>
+      </c>
+      <c r="E5">
+        <v>0.40912892935754369</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E6">
+        <v>369.08323917404419</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7">
+        <v>1</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
+      <c r="D7">
+        <v>1</v>
+      </c>
+      <c r="E7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8">
+        <v>1</v>
+      </c>
+      <c r="C8">
+        <v>0</v>
+      </c>
+      <c r="D8">
+        <v>0</v>
+      </c>
+      <c r="E8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9">
+        <v>32.984378932490898</v>
+      </c>
+      <c r="C9">
+        <v>3.000070688235291</v>
+      </c>
+      <c r="D9">
+        <v>62.437884687648456</v>
+      </c>
+      <c r="E9">
+        <v>420.81949491143354</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E10">
+        <v>3.2336185741314547</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>